<commit_message>
Updating screenshot utility and writing table to excel
</commit_message>
<xml_diff>
--- a/src/main/java/Org/testdata/TestDataAdactin.xlsx
+++ b/src/main/java/Org/testdata/TestDataAdactin.xlsx
@@ -3,21 +3,18 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Eclipse\Workspace\MAvenProject\src\main\java\Org\testdata\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9B43C17-9B16-4A30-A51F-D17FCD14A340}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{9ED69F41-F1F6-4DBF-BD51-3AAEA7610EEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2544" yWindow="2544" windowWidth="17280" windowHeight="5460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="23280" windowHeight="13224" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SearchPage" sheetId="1" r:id="rId1"/>
+    <sheet name="BookingHistory" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:K28"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
   <si>
     <t>Location</t>
   </si>
@@ -109,12 +106,28 @@
   </si>
   <si>
     <t>1 - One</t>
+  </si>
+  <si>
+    <t>Order Id</t>
+  </si>
+  <si>
+    <t>Total Price</t>
+  </si>
+  <si>
+    <t>URXJ1F704M</t>
+  </si>
+  <si>
+    <t>AUD $ 396</t>
+  </si>
+  <si>
+    <t>Z2U1I9YV37</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -152,10 +165,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,14 +453,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="13.109375" collapsed="true"/>
+    <col min="5" max="6" bestFit="true" customWidth="true" width="10.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -582,4 +597,45 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.83984375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.53125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>